<commit_message>
added sql and schemas
</commit_message>
<xml_diff>
--- a/docs/project_semester_variants.xlsx
+++ b/docs/project_semester_variants.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anka\Desktop\studia\sem3\Database Systems\lecture\project_DBS\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EA03EB-5229-4B85-B1A3-BF7F98DE4E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -355,7 +361,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -373,12 +379,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -408,14 +420,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -423,14 +436,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -468,7 +484,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -540,7 +556,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -713,19 +729,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="53.77734375" customWidth="1"/>
-    <col min="3" max="3" width="48.5546875" customWidth="1"/>
+    <col min="2" max="2" width="53.81640625" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" customWidth="1"/>
     <col min="4" max="4" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -739,7 +757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -753,7 +771,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -767,7 +785,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -781,7 +799,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -795,21 +813,21 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -823,7 +841,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -837,7 +855,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -851,7 +869,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -865,7 +883,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -879,7 +897,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -893,7 +911,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -907,7 +925,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -921,7 +939,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -935,7 +953,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -949,7 +967,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -963,7 +981,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -977,7 +995,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -991,7 +1009,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1005,7 +1023,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1019,7 +1037,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1033,7 +1051,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1047,7 +1065,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1061,7 +1079,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1075,7 +1093,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1089,7 +1107,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1103,7 +1121,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1117,7 +1135,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1131,7 +1149,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1145,7 +1163,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1159,7 +1177,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1173,7 +1191,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1187,7 +1205,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1201,7 +1219,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1215,7 +1233,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1229,7 +1247,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1243,7 +1261,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1257,7 +1275,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1271,7 +1289,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1285,7 +1303,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1299,7 +1317,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1313,7 +1331,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1327,7 +1345,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1341,7 +1359,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1355,7 +1373,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1369,7 +1387,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1383,7 +1401,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1397,7 +1415,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1411,7 +1429,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1425,7 +1443,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1439,7 +1457,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1453,7 +1471,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1467,7 +1485,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1481,7 +1499,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1495,7 +1513,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1509,7 +1527,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1523,7 +1541,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1537,7 +1555,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1551,7 +1569,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1565,7 +1583,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1579,7 +1597,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1593,7 +1611,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1607,7 +1625,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1621,7 +1639,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1635,7 +1653,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1649,7 +1667,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1663,7 +1681,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1677,7 +1695,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1691,7 +1709,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1705,7 +1723,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1719,7 +1737,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1733,7 +1751,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1747,7 +1765,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1761,7 +1779,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1775,7 +1793,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1789,7 +1807,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1803,7 +1821,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1817,7 +1835,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1831,7 +1849,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1845,7 +1863,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>

</xml_diff>